<commit_message>
Add fines functionality and related changes
</commit_message>
<xml_diff>
--- a/scripts/Clean.xlsx
+++ b/scripts/Clean.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Car Name</t>
   </si>
@@ -46,52 +46,31 @@
     <t>Dispute</t>
   </si>
   <si>
-    <t>FORD MUSTANG, 2024, Black</t>
-  </si>
-  <si>
-    <t>BMW 330I 2023, Black</t>
-  </si>
-  <si>
-    <t>NISSAN SENTRA, 2023, Blue</t>
+    <t>CADILLAC ESCALADE, 2023, Blue</t>
   </si>
   <si>
     <t>KIA K5, 2023, Black</t>
   </si>
   <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CC</t>
+    <t>N</t>
   </si>
   <si>
     <t>DD</t>
   </si>
   <si>
-    <t>57782</t>
-  </si>
-  <si>
-    <t>30526</t>
-  </si>
-  <si>
-    <t>37961</t>
+    <t>85540</t>
   </si>
   <si>
     <t>81392</t>
   </si>
   <si>
-    <t>12 Jul 2025, 4:58 am</t>
-  </si>
-  <si>
-    <t>12 Jul 2025, 3:41 am</t>
-  </si>
-  <si>
-    <t>11 Jul 2025, 1:18 pm</t>
+    <t>14 Jul 2025, 12:10 am</t>
   </si>
   <si>
     <t>11 Jul 2025, 8:30 am</t>
   </si>
   <si>
-    <t>Sheikh Zayed Road</t>
+    <t>Ras Al khour St</t>
   </si>
   <si>
     <t>Dubai Alain Road</t>
@@ -100,34 +79,16 @@
     <t>Dubai Police</t>
   </si>
   <si>
-    <t>AED 700</t>
-  </si>
-  <si>
     <t>AED 600</t>
   </si>
   <si>
-    <t>AED 400</t>
-  </si>
-  <si>
-    <t>7037849083</t>
-  </si>
-  <si>
-    <t>7037848839</t>
-  </si>
-  <si>
-    <t>7037858268</t>
+    <t>7037866556</t>
   </si>
   <si>
     <t>7037841032</t>
   </si>
   <si>
-    <t>Exceeding maximum speed limit by not more than 40 km h</t>
-  </si>
-  <si>
     <t>Exceeding maximum speed limit by not more than 30 km h</t>
-  </si>
-  <si>
-    <t>failure of a light vehicle to abid by lane discipline</t>
   </si>
   <si>
     <t>Please contact Dubai Police for details about disputing your fine.</t>
@@ -488,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -531,31 +492,31 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -563,95 +524,31 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>